<commit_message>
Added one extra ethnicity label.
</commit_message>
<xml_diff>
--- a/ethnicity_groups.xlsx
+++ b/ethnicity_groups.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/pml204_exeter_ac_uk/Documents/Documents/mody/Pedro/Paper Writing - Clinical Paper/Julieanne-Pedro-MODY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C745FC2-0FA8-4FA0-BC7C-2F330FFD9ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{8C745FC2-0FA8-4FA0-BC7C-2F330FFD9ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FE2521A-2B94-4821-80C3-1DBD48B283D1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="12600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ethnicity_groups" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="281">
   <si>
     <t>Ethnicity</t>
   </si>
@@ -860,12 +860,15 @@
   </si>
   <si>
     <t>Māori</t>
+  </si>
+  <si>
+    <t>British Asian/Pakistani</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1699,11 +1702,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C278"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="C284" sqref="C284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4769,6 +4772,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>280</v>
+      </c>
+      <c r="B279">
+        <v>1</v>
+      </c>
+      <c r="C279">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>